<commit_message>
requirements and some debugging
</commit_message>
<xml_diff>
--- a/expense_report.xlsx
+++ b/expense_report.xlsx
@@ -236,7 +236,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +248,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -476,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,7 +496,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -598,13 +604,13 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -709,11 +715,8 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1029,19 +1032,19 @@
     <col min="1" max="1" style="76" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="76" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="77" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="78" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="78" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="78" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="78" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="78" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="78" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="78" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="78" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="79" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="80" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="77" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="77" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="77" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="77" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="77" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="77" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="77" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="77" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="78" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="79" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -1075,7 +1078,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1094,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="42">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="40.5">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -1161,7 +1164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="53.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="51.75">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
@@ -1196,7 +1199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="26"/>
       <c r="B8" s="27"/>
       <c r="C8" s="28"/>
@@ -1229,7 +1232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="31" t="s">
         <v>22</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="32">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="32">
       <c r="A10" s="33"/>
       <c r="B10" s="34"/>
       <c r="C10" s="28" t="s">
@@ -1275,7 +1278,7 @@
       <c r="L10" s="35"/>
       <c r="M10" s="36"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="32">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="32">
       <c r="A11" s="33"/>
       <c r="B11" s="9" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
centered and top align form fields in template
</commit_message>
<xml_diff>
--- a/expense_report.xlsx
+++ b/expense_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chadthompsonsmith/Oracle_Cloud/expense_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A71021-7FAE-704C-8236-8B6C9256F6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45464495-E9B7-654C-AD13-E432A9D44B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="-11400" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,7 +616,91 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -624,10 +708,25 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -637,14 +736,20 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -652,131 +757,29 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,7 +1089,7 @@
   <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E6"/>
+      <selection activeCell="H5" sqref="H5:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1100,19 +1103,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4" t="s">
         <v>1</v>
@@ -1155,20 +1158,20 @@
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="79" t="s">
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="90"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="93"/>
       <c r="L4" s="7">
         <v>2</v>
       </c>
@@ -1180,18 +1183,18 @@
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="80" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="70"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
       <c r="L5" s="7">
         <v>3</v>
       </c>
@@ -1201,16 +1204,16 @@
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
       <c r="L6" s="7">
         <v>4</v>
       </c>
@@ -1219,9 +1222,9 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="59"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
@@ -1243,7 +1246,7 @@
       <c r="J7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="51" t="s">
         <v>17</v>
       </c>
       <c r="L7" s="7">
@@ -1254,9 +1257,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="65"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="67"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="13" t="s">
         <v>19</v>
       </c>
@@ -1278,7 +1281,7 @@
       <c r="J8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="85"/>
+      <c r="K8" s="52"/>
       <c r="L8" s="7">
         <v>6</v>
       </c>
@@ -1287,10 +1290,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="58" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -1315,8 +1318,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="76"/>
-      <c r="B10" s="75"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="12" t="s">
         <v>25</v>
       </c>
@@ -1335,11 +1338,11 @@
       <c r="M10" s="17"/>
     </row>
     <row r="11" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="76"/>
-      <c r="B11" s="68" t="s">
+      <c r="A11" s="59"/>
+      <c r="B11" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1355,11 +1358,11 @@
       <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="76"/>
-      <c r="B12" s="68" t="s">
+      <c r="A12" s="59"/>
+      <c r="B12" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -1375,11 +1378,11 @@
       <c r="M12" s="17"/>
     </row>
     <row r="13" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="76"/>
-      <c r="B13" s="68" t="s">
+      <c r="A13" s="59"/>
+      <c r="B13" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="70"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -1395,11 +1398,11 @@
       <c r="M13" s="17"/>
     </row>
     <row r="14" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="76"/>
-      <c r="B14" s="68" t="s">
+      <c r="A14" s="59"/>
+      <c r="B14" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="70"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -1415,11 +1418,11 @@
       <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="76"/>
-      <c r="B15" s="68" t="s">
+      <c r="A15" s="59"/>
+      <c r="B15" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="70"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -1435,11 +1438,11 @@
       <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="75"/>
-      <c r="B16" s="68" t="s">
+      <c r="A16" s="60"/>
+      <c r="B16" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="70"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -1455,13 +1458,13 @@
       <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="70"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -1477,11 +1480,11 @@
       <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="75"/>
-      <c r="B18" s="68" t="s">
+      <c r="A18" s="60"/>
+      <c r="B18" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="70"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -1497,13 +1500,13 @@
       <c r="M18" s="17"/>
     </row>
     <row r="19" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="70"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -1519,11 +1522,11 @@
       <c r="M19" s="17"/>
     </row>
     <row r="20" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="76"/>
-      <c r="B20" s="68" t="s">
+      <c r="A20" s="59"/>
+      <c r="B20" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="70"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -1539,11 +1542,11 @@
       <c r="M20" s="17"/>
     </row>
     <row r="21" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="75"/>
-      <c r="B21" s="68" t="s">
+      <c r="A21" s="60"/>
+      <c r="B21" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="70"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1559,13 +1562,13 @@
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="70"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -1581,11 +1584,11 @@
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="75"/>
-      <c r="B23" s="68" t="s">
+      <c r="A23" s="60"/>
+      <c r="B23" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="70"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1601,13 +1604,13 @@
       <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="70"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1623,11 +1626,11 @@
       <c r="M24" s="17"/>
     </row>
     <row r="25" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="76"/>
-      <c r="B25" s="68" t="s">
+      <c r="A25" s="59"/>
+      <c r="B25" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="70"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1643,11 +1646,11 @@
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="76"/>
-      <c r="B26" s="68" t="s">
+      <c r="A26" s="59"/>
+      <c r="B26" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="70"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1663,11 +1666,11 @@
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="75"/>
-      <c r="B27" s="68" t="s">
+      <c r="A27" s="60"/>
+      <c r="B27" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="70"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12" t="s">
         <v>19</v>
@@ -1685,11 +1688,11 @@
       <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="70"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="12">
         <f t="shared" ref="D28:K28" si="1">SUM(D10:D27)</f>
         <v>0</v>
@@ -1733,11 +1736,11 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
-      <c r="H29" s="71" t="s">
+      <c r="H29" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="I29" s="72"/>
-      <c r="J29" s="73"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="65"/>
       <c r="K29" s="12"/>
       <c r="L29" s="3"/>
     </row>
@@ -1751,11 +1754,11 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="71" t="s">
+      <c r="H30" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="72"/>
-      <c r="J30" s="73"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="65"/>
       <c r="K30" s="12"/>
       <c r="L30" s="3"/>
     </row>
@@ -1767,11 +1770,11 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="71" t="s">
+      <c r="H31" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="72"/>
-      <c r="J31" s="73"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="65"/>
       <c r="K31" s="12">
         <f>IF(K28&lt;K29,(K29-K30-K28),0)</f>
         <v>0</v>
@@ -1786,11 +1789,11 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="71" t="s">
+      <c r="H32" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="I32" s="72"/>
-      <c r="J32" s="73"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="65"/>
       <c r="K32" s="12">
         <f>IF(K28&gt;K29,(K28-K30-K29),0)</f>
         <v>0</v>
@@ -1813,19 +1816,19 @@
       <c r="M33" s="17"/>
     </row>
     <row r="34" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="41"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="69"/>
       <c r="L34" s="16"/>
       <c r="M34" s="17"/>
     </row>
@@ -1833,18 +1836,18 @@
       <c r="A35" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="64" t="s">
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="40"/>
-      <c r="I35" s="41"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="69"/>
       <c r="J35" s="12" t="s">
         <v>57</v>
       </c>
@@ -1856,56 +1859,56 @@
     </row>
     <row r="36" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="23"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="63"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="42"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="63"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="42"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="63"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="42"/>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="62"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="62"/>
-      <c r="I39" s="63"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="42"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="3"/>
@@ -1925,21 +1928,21 @@
       <c r="L40" s="3"/>
     </row>
     <row r="41" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="57" t="s">
+      <c r="B41" s="67"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="59"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="83"/>
+      <c r="J41" s="83"/>
+      <c r="K41" s="47"/>
       <c r="L41" s="16"/>
       <c r="M41" s="17"/>
     </row>
@@ -1947,112 +1950,112 @@
       <c r="A42" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="50"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="85"/>
       <c r="F42" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="57" t="s">
+      <c r="G42" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="H42" s="60"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="61"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="86"/>
+      <c r="J42" s="86"/>
+      <c r="K42" s="87"/>
       <c r="L42" s="3"/>
     </row>
     <row r="43" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="23"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="25"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="55"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="75"/>
       <c r="L43" s="3"/>
     </row>
     <row r="44" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="23"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="41"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="69"/>
       <c r="F44" s="25"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="53"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="80"/>
+      <c r="I44" s="80"/>
+      <c r="J44" s="80"/>
+      <c r="K44" s="81"/>
       <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="41"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="69"/>
       <c r="F45" s="25"/>
-      <c r="G45" s="54" t="s">
+      <c r="G45" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="55"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="74"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="75"/>
       <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="41"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="68"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="69"/>
       <c r="F46" s="25"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="55"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="75"/>
       <c r="L46" s="3"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="41"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="69"/>
       <c r="F47" s="25"/>
-      <c r="G47" s="42" t="s">
+      <c r="G47" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="42"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="74"/>
+      <c r="J47" s="74"/>
+      <c r="K47" s="74"/>
       <c r="L47" s="3"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="41"/>
+      <c r="B48" s="66"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="69"/>
       <c r="F48" s="25"/>
-      <c r="G48" s="43" t="s">
+      <c r="G48" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="45"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77"/>
+      <c r="J48" s="77"/>
+      <c r="K48" s="78"/>
       <c r="L48" s="3"/>
     </row>
     <row r="49" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2208,56 +2211,6 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="H5:K6"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="G43:K43"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="G39:I39"/>
     <mergeCell ref="B47:E47"/>
     <mergeCell ref="G47:K47"/>
     <mergeCell ref="B48:E48"/>
@@ -2268,10 +2221,60 @@
     <mergeCell ref="G45:K45"/>
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="G46:K46"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="G43:K43"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="G39:I39"/>
     <mergeCell ref="A41:F41"/>
     <mergeCell ref="G41:K41"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="G42:K42"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="H5:K6"/>
+    <mergeCell ref="B5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more merge center edits on form fields
</commit_message>
<xml_diff>
--- a/expense_report.xlsx
+++ b/expense_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chadthompsonsmith/Oracle_Cloud/expense_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45464495-E9B7-654C-AD13-E432A9D44B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF26B2F-1AF8-DA4B-8E23-B1160A27390D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="-11400" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,9 +526,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -616,6 +613,114 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,31 +730,13 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -658,8 +745,23 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -673,113 +775,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,28 +1094,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="10.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="10.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="37" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
+      <c r="A1" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4" t="s">
         <v>1</v>
@@ -1158,20 +1158,20 @@
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="41" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="93"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="84"/>
       <c r="L4" s="7">
         <v>2</v>
       </c>
@@ -1179,22 +1179,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="43" t="s">
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
       <c r="L5" s="7">
         <v>3</v>
       </c>
@@ -1203,17 +1203,17 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
       <c r="L6" s="7">
         <v>4</v>
       </c>
@@ -1222,31 +1222,31 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="10" t="s">
+      <c r="A7" s="77"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="51" t="s">
+      <c r="K7" s="80" t="s">
         <v>17</v>
       </c>
       <c r="L7" s="7">
@@ -1257,31 +1257,31 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="13" t="s">
+      <c r="A8" s="62"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="52"/>
+      <c r="K8" s="81"/>
       <c r="L8" s="7">
         <v>6</v>
       </c>
@@ -1290,23 +1290,23 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11">
         <f t="shared" ref="K9:K27" si="0">SUM(D9:J9)</f>
         <v>0</v>
       </c>
@@ -1317,431 +1317,431 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="59"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="12" t="s">
+    <row r="10" spans="1:13" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="73"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17"/>
-    </row>
-    <row r="11" spans="1:13" s="14" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
-      <c r="B11" s="61" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="73"/>
+      <c r="B11" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12">
+      <c r="C11" s="67"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
-    </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
-      <c r="B12" s="61" t="s">
+      <c r="L11" s="15"/>
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="73"/>
+      <c r="B12" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12">
+      <c r="C12" s="67"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
-    </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59"/>
-      <c r="B13" s="61" t="s">
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="73"/>
+      <c r="B13" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12">
+      <c r="C13" s="67"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17"/>
-    </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="59"/>
-      <c r="B14" s="61" t="s">
+      <c r="L13" s="15"/>
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="73"/>
+      <c r="B14" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12">
+      <c r="C14" s="67"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="17"/>
-    </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="59"/>
-      <c r="B15" s="61" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="73"/>
+      <c r="B15" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12">
+      <c r="C15" s="67"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
-    </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
-      <c r="B16" s="61" t="s">
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="72"/>
+      <c r="B16" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12">
+      <c r="C16" s="67"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="17"/>
-    </row>
-    <row r="17" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="58" t="s">
+      <c r="L16" s="15"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12">
+      <c r="C17" s="67"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="17"/>
-    </row>
-    <row r="18" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
-      <c r="B18" s="61" t="s">
+      <c r="L17" s="15"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="72"/>
+      <c r="B18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12">
+      <c r="C18" s="67"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="17"/>
-    </row>
-    <row r="19" spans="1:13" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="58" t="s">
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
+    </row>
+    <row r="19" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12">
+      <c r="C19" s="67"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="17"/>
-    </row>
-    <row r="20" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59"/>
-      <c r="B20" s="61" t="s">
+      <c r="L19" s="15"/>
+      <c r="M19" s="16"/>
+    </row>
+    <row r="20" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="73"/>
+      <c r="B20" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12">
+      <c r="C20" s="67"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="17"/>
-    </row>
-    <row r="21" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
-      <c r="B21" s="61" t="s">
+      <c r="L20" s="15"/>
+      <c r="M20" s="16"/>
+    </row>
+    <row r="21" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="72"/>
+      <c r="B21" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12">
+      <c r="C21" s="67"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L21" s="16"/>
-      <c r="M21" s="17"/>
-    </row>
-    <row r="22" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="58" t="s">
+      <c r="L21" s="15"/>
+      <c r="M21" s="16"/>
+    </row>
+    <row r="22" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12">
+      <c r="C22" s="67"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L22" s="16"/>
-      <c r="M22" s="17"/>
-    </row>
-    <row r="23" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
-      <c r="B23" s="61" t="s">
+      <c r="L22" s="15"/>
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="72"/>
+      <c r="B23" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12">
+      <c r="C23" s="67"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="17"/>
-    </row>
-    <row r="24" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="58" t="s">
+      <c r="L23" s="15"/>
+      <c r="M23" s="16"/>
+    </row>
+    <row r="24" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12">
+      <c r="C24" s="67"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="17"/>
-    </row>
-    <row r="25" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="59"/>
-      <c r="B25" s="61" t="s">
+      <c r="L24" s="15"/>
+      <c r="M24" s="16"/>
+    </row>
+    <row r="25" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="73"/>
+      <c r="B25" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12">
+      <c r="C25" s="67"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L25" s="16"/>
-      <c r="M25" s="17"/>
-    </row>
-    <row r="26" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="59"/>
-      <c r="B26" s="61" t="s">
+      <c r="L25" s="15"/>
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="73"/>
+      <c r="B26" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12">
+      <c r="C26" s="67"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L26" s="16"/>
-      <c r="M26" s="17"/>
-    </row>
-    <row r="27" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
-      <c r="B27" s="61" t="s">
+      <c r="L26" s="15"/>
+      <c r="M26" s="16"/>
+    </row>
+    <row r="27" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="72"/>
+      <c r="B27" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12" t="s">
+      <c r="C27" s="67"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12">
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="17"/>
-    </row>
-    <row r="28" spans="1:13" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="61" t="s">
+      <c r="L27" s="15"/>
+      <c r="M27" s="16"/>
+    </row>
+    <row r="28" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="62"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="12">
+      <c r="B28" s="66"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="11">
         <f t="shared" ref="D28:K28" si="1">SUM(D10:D27)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="17"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="63" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="I29" s="64"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="12"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="11"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1754,12 +1754,12 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="63" t="s">
+      <c r="H30" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="64"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="12"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1770,12 +1770,12 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="63" t="s">
+      <c r="H31" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="64"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="12">
+      <c r="I31" s="69"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="11">
         <f>IF(K28&lt;K29,(K29-K30-K28),0)</f>
         <v>0</v>
       </c>
@@ -1789,128 +1789,128 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="63" t="s">
+      <c r="H32" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="I32" s="64"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="12">
+      <c r="I32" s="69"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="11">
         <f>IF(K28&gt;K29,(K28-K30-K29),0)</f>
         <v>0</v>
       </c>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:13" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="17"/>
-    </row>
-    <row r="34" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="66" t="s">
+    <row r="33" spans="1:13" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="16"/>
+    </row>
+    <row r="34" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="67"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="17"/>
-    </row>
-    <row r="35" spans="1:13" s="14" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
+      <c r="B34" s="53"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="16"/>
+    </row>
+    <row r="35" spans="1:13" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="71" t="s">
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="68"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="12" t="s">
+      <c r="H35" s="39"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="K35" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L35" s="16"/>
-      <c r="M35" s="17"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="16"/>
     </row>
     <row r="36" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
       <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="66"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
       <c r="L39" s="3"/>
     </row>
     <row r="40" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1927,181 +1927,181 @@
       <c r="K40" s="6"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="66" t="s">
+    <row r="41" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="67"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="82" t="s">
+      <c r="B41" s="53"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="83"/>
-      <c r="I41" s="83"/>
-      <c r="J41" s="83"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="17"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="56"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="16"/>
     </row>
     <row r="42" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="53" t="s">
+      <c r="B42" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="84"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="22" t="s">
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="82" t="s">
+      <c r="G42" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="H42" s="86"/>
-      <c r="I42" s="86"/>
-      <c r="J42" s="86"/>
-      <c r="K42" s="87"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="61"/>
       <c r="L42" s="3"/>
     </row>
     <row r="43" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="23"/>
-      <c r="B43" s="66"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="75"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="49"/>
       <c r="L43" s="3"/>
     </row>
     <row r="44" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="23"/>
-      <c r="B44" s="66"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="79"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="80"/>
-      <c r="J44" s="80"/>
-      <c r="K44" s="81"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="47"/>
       <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="66"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="73" t="s">
+      <c r="A45" s="14"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="75"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="49"/>
       <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
-      <c r="B46" s="66"/>
-      <c r="C46" s="68"/>
-      <c r="D46" s="68"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="75"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="49"/>
       <c r="L46" s="3"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="15"/>
-      <c r="B47" s="66"/>
-      <c r="C47" s="68"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="74" t="s">
+      <c r="A47" s="14"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="74"/>
-      <c r="K47" s="74"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="41"/>
       <c r="L47" s="3"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="15"/>
-      <c r="B48" s="66"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="76" t="s">
+      <c r="A48" s="14"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="H48" s="77"/>
-      <c r="I48" s="77"/>
-      <c r="J48" s="77"/>
-      <c r="K48" s="78"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="44"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="17"/>
-    </row>
-    <row r="50" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="17"/>
-    </row>
-    <row r="51" spans="1:13" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="28"/>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="17"/>
+    <row r="49" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="16"/>
+    </row>
+    <row r="50" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="16"/>
+    </row>
+    <row r="51" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="25"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="16"/>
     </row>
     <row r="52" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
@@ -2118,11 +2118,11 @@
       <c r="L52" s="3"/>
     </row>
     <row r="53" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="24"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="23"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -2134,11 +2134,11 @@
       <c r="L53" s="3"/>
     </row>
     <row r="54" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B54" s="5"/>
-      <c r="C54" s="32">
+      <c r="C54" s="31">
         <f>SUM(K10:K21)</f>
         <v>0</v>
       </c>
@@ -2153,11 +2153,11 @@
       <c r="L54" s="3"/>
     </row>
     <row r="55" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="5"/>
-      <c r="C55" s="32">
+      <c r="C55" s="31">
         <f>SUM(K22:K23)</f>
         <v>0</v>
       </c>
@@ -2172,11 +2172,11 @@
       <c r="L55" s="3"/>
     </row>
     <row r="56" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="30" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="5"/>
-      <c r="C56" s="32">
+      <c r="C56" s="31">
         <f>+K24</f>
         <v>0</v>
       </c>
@@ -2191,11 +2191,11 @@
       <c r="L56" s="3"/>
     </row>
     <row r="57" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="34"/>
-      <c r="C57" s="35">
+      <c r="B57" s="33"/>
+      <c r="C57" s="34">
         <f>+K25</f>
         <v>0</v>
       </c>
@@ -2210,17 +2210,50 @@
       <c r="L57" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="G44:K44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="G45:K45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="G46:K46"/>
+  <mergeCells count="65">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="H5:K6"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="G36:I36"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="G43:K43"/>
     <mergeCell ref="B37:F37"/>
@@ -2233,48 +2266,16 @@
     <mergeCell ref="G41:K41"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="G42:K42"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="H5:K6"/>
-    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G48:K48"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="G45:K45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="G46:K46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated nginx proxy readme and instructions with new youtube link
</commit_message>
<xml_diff>
--- a/expense_report.xlsx
+++ b/expense_report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chadthompsonsmith/Oracle_Cloud/expense_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF26B2F-1AF8-DA4B-8E23-B1160A27390D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843BC6BA-A7A5-9642-9681-8CC3AA8A7574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="-11400" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,7 +613,109 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -621,10 +723,46 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -642,144 +780,6 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1085,11 +1085,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:K6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1103,19 +1104,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4" t="s">
         <v>1</v>
@@ -1158,20 +1159,20 @@
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="76" t="s">
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="84"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="7">
         <v>2</v>
       </c>
@@ -1180,21 +1181,21 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="92" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="92"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
       <c r="L5" s="7">
         <v>3</v>
       </c>
@@ -1203,17 +1204,17 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
       <c r="L6" s="7">
         <v>4</v>
       </c>
@@ -1222,9 +1223,9 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="56"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="9" t="s">
         <v>10</v>
       </c>
@@ -1246,7 +1247,7 @@
       <c r="J7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="80" t="s">
+      <c r="K7" s="48" t="s">
         <v>17</v>
       </c>
       <c r="L7" s="7">
@@ -1257,9 +1258,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="62"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="64"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="12" t="s">
         <v>19</v>
       </c>
@@ -1281,7 +1282,7 @@
       <c r="J8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="81"/>
+      <c r="K8" s="49"/>
       <c r="L8" s="7">
         <v>6</v>
       </c>
@@ -1290,10 +1291,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="62" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1318,8 +1319,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="73"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="64"/>
       <c r="C10" s="11" t="s">
         <v>25</v>
       </c>
@@ -1338,11 +1339,11 @@
       <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="73"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1358,11 +1359,11 @@
       <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="73"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1378,11 +1379,11 @@
       <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="73"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -1398,11 +1399,11 @@
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="73"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="67"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1418,11 +1419,11 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="73"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -1438,11 +1439,11 @@
       <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="72"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="67"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -1458,13 +1459,13 @@
       <c r="M16" s="16"/>
     </row>
     <row r="17" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="62" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="67"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -1480,11 +1481,11 @@
       <c r="M17" s="16"/>
     </row>
     <row r="18" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="72"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="67"/>
+      <c r="C18" s="66"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -1500,13 +1501,13 @@
       <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="62" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="67"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -1522,11 +1523,11 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="73"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="67"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1542,11 +1543,11 @@
       <c r="M20" s="16"/>
     </row>
     <row r="21" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="72"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="67"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -1562,13 +1563,13 @@
       <c r="M21" s="16"/>
     </row>
     <row r="22" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="62" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="67"/>
+      <c r="C22" s="66"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -1584,11 +1585,11 @@
       <c r="M22" s="16"/>
     </row>
     <row r="23" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="72"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="67"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -1604,13 +1605,13 @@
       <c r="M23" s="16"/>
     </row>
     <row r="24" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="62" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="67"/>
+      <c r="C24" s="66"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
@@ -1626,11 +1627,11 @@
       <c r="M24" s="16"/>
     </row>
     <row r="25" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="73"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="67"/>
+      <c r="C25" s="66"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
@@ -1646,11 +1647,11 @@
       <c r="M25" s="16"/>
     </row>
     <row r="26" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="67"/>
+      <c r="C26" s="66"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -1666,11 +1667,11 @@
       <c r="M26" s="16"/>
     </row>
     <row r="27" spans="1:13" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="72"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="67"/>
+      <c r="C27" s="66"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11" t="s">
         <v>19</v>
@@ -1691,8 +1692,8 @@
       <c r="A28" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="67"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="66"/>
       <c r="D28" s="11">
         <f t="shared" ref="D28:K28" si="1">SUM(D10:D27)</f>
         <v>0</v>
@@ -1816,19 +1817,19 @@
       <c r="M33" s="16"/>
     </row>
     <row r="34" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="53"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="40"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="74"/>
       <c r="L34" s="15"/>
       <c r="M34" s="16"/>
     </row>
@@ -1836,18 +1837,18 @@
       <c r="A35" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="52" t="s">
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="74"/>
       <c r="J35" s="11" t="s">
         <v>57</v>
       </c>
@@ -1859,56 +1860,56 @@
     </row>
     <row r="36" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="51"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="41"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="51"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="41"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="51"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="41"/>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="51"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="41"/>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
       <c r="L39" s="3"/>
@@ -1928,21 +1929,21 @@
       <c r="L40" s="3"/>
     </row>
     <row r="41" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="54" t="s">
+      <c r="B41" s="72"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="56"/>
+      <c r="H41" s="82"/>
+      <c r="I41" s="82"/>
+      <c r="J41" s="82"/>
+      <c r="K41" s="44"/>
       <c r="L41" s="15"/>
       <c r="M41" s="16"/>
     </row>
@@ -1950,112 +1951,112 @@
       <c r="A42" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="59"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="85"/>
       <c r="F42" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="54" t="s">
+      <c r="G42" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="H42" s="60"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="61"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="86"/>
+      <c r="J42" s="86"/>
+      <c r="K42" s="87"/>
       <c r="L42" s="3"/>
     </row>
     <row r="43" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="40"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="74"/>
       <c r="F43" s="24"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="49"/>
+      <c r="G43" s="78"/>
+      <c r="H43" s="79"/>
+      <c r="I43" s="79"/>
+      <c r="J43" s="79"/>
+      <c r="K43" s="80"/>
       <c r="L43" s="3"/>
     </row>
     <row r="44" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="22"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="40"/>
+      <c r="B44" s="71"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="74"/>
       <c r="F44" s="24"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="47"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="92"/>
+      <c r="K44" s="93"/>
       <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="40"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="74"/>
       <c r="F45" s="24"/>
-      <c r="G45" s="48" t="s">
+      <c r="G45" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="49"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="80"/>
       <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="40"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="74"/>
       <c r="F46" s="24"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="49"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="79"/>
+      <c r="K46" s="80"/>
       <c r="L46" s="3"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="40"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="74"/>
       <c r="F47" s="24"/>
-      <c r="G47" s="41" t="s">
+      <c r="G47" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41"/>
+      <c r="H47" s="79"/>
+      <c r="I47" s="79"/>
+      <c r="J47" s="79"/>
+      <c r="K47" s="79"/>
       <c r="L47" s="3"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="40"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="74"/>
       <c r="F48" s="24"/>
-      <c r="G48" s="42" t="s">
+      <c r="G48" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="44"/>
+      <c r="H48" s="89"/>
+      <c r="I48" s="89"/>
+      <c r="J48" s="89"/>
+      <c r="K48" s="90"/>
       <c r="L48" s="3"/>
     </row>
     <row r="49" spans="1:13" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2211,49 +2212,16 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="H5:K6"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G48:K48"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="G45:K45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="G46:K46"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="G43:K43"/>
     <mergeCell ref="B37:F37"/>
@@ -2266,18 +2234,52 @@
     <mergeCell ref="G41:K41"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="G42:K42"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="G48:K48"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="G44:K44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="G45:K45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="H5:K6"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="F5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="66" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2293,6 +2295,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2308,5 +2311,6 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>